<commit_message>
adicionado classe para gerenciar template em planilhas
</commit_message>
<xml_diff>
--- a/src/main/resources/pessoas.xlsx
+++ b/src/main/resources/pessoas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22505"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A78DFDE3-74C7-4719-B833-1A6B65A2E83B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -24,8 +24,46 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Autor</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:area(lastCell="B2")
+jx:each(items="pessoas" groupBy="name" lastCell="B2")
+jx:each(items="_group.items" var="pessoas" lastCell="B1")</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Nome</t>
   </si>
@@ -55,13 +93,16 @@
   </si>
   <si>
     <t>Santos</t>
+  </si>
+  <si>
+    <t>${pessoas}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,6 +117,21 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -411,28 +467,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="A4:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -449,7 +505,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -466,7 +522,7 @@
         <v>33988</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -486,4 +542,28 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>